<commit_message>
[BE] import file: change to Vietnamese template
</commit_message>
<xml_diff>
--- a/packages/backend_php/public/templates/TopicTemplate.xlsx
+++ b/packages/backend_php/public/templates/TopicTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quang\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HOC-TAP\KLTN\source\packages\backend_php\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4002FA69-6342-400B-B0CA-E9588A5AE5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BA792F-3E05-4675-BD82-A2B1EDC9AF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{9DEBA3BE-0AFB-4864-9C29-2007BD4153E4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{9DEBA3BE-0AFB-4864-9C29-2007BD4153E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,31 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Code(*)</t>
-  </si>
-  <si>
-    <t>Title(*)</t>
-  </si>
-  <si>
-    <t>Limit(*)</t>
-  </si>
-  <si>
-    <t>Thesis Defense Date</t>
-  </si>
-  <si>
-    <t>Schedule Code</t>
-  </si>
-  <si>
-    <t>Lecturer Code</t>
-  </si>
-  <si>
-    <t>Critical Code</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Xây dựng hệ thống nhận diện chó </t>
   </si>
@@ -69,15 +45,43 @@
   </si>
   <si>
     <t>2023-KL-001</t>
+  </si>
+  <si>
+    <t>Mã đề tài(*)</t>
+  </si>
+  <si>
+    <t>Tiêu đề(*)</t>
+  </si>
+  <si>
+    <t>Mã đợt</t>
+  </si>
+  <si>
+    <t>Mã GVHD</t>
+  </si>
+  <si>
+    <t>Số lượng SV(*)</t>
+  </si>
+  <si>
+    <t>Mã GVPB</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -127,14 +131,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,60 +453,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680E96E1-88E2-47E4-AC90-38D7E9321D6A}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8" style="3" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18" style="3" customWidth="1"/>
-    <col min="8" max="8" width="44.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="4" customWidth="1"/>
+    <col min="4" max="6" width="18.77734375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="61.33203125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>